<commit_message>
Started on batch styles processing
</commit_message>
<xml_diff>
--- a/data/reports.xlsx
+++ b/data/reports.xlsx
@@ -5,8 +5,8 @@
     <workbookView tabRatio="600" windowHeight="14980" windowWidth="25600" xWindow="0" yWindow="1080"/>
   </bookViews>
   <sheets>
-    <sheet name="monthlySummary" sheetId="1" r:id="RHbx6zqMXm2SS9GRf"/>
-    <sheet name="monthlyDetail" sheetId="2" r:id="R9GYCLqw71EMf7IQq"/>
+    <sheet name="monthlySummary" sheetId="1" r:id="RRvNqx4YwEJikCvdm"/>
+    <sheet name="monthlyDetail" sheetId="2" r:id="R2RXQrW0gJizUtVFE"/>
   </sheets>
 </workbook>
 </file>

</xml_diff>